<commit_message>
added very simple sensor model with observation probabilities
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/mannedShipTestOutput.xlsx
+++ b/shipClassTests/testResults/mannedShipTestOutput.xlsx
@@ -555,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -575,7 +575,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -615,10 +615,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -632,19 +632,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -652,19 +652,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -672,19 +672,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -692,19 +692,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -712,19 +712,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -732,19 +732,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -755,16 +755,16 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -775,16 +775,16 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -795,16 +795,16 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -815,16 +815,16 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -835,16 +835,16 @@
         <v>2</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -855,16 +855,16 @@
         <v>2</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -875,16 +875,16 @@
         <v>2</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -895,16 +895,16 @@
         <v>2</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -915,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F24" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -932,19 +932,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -952,19 +952,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -972,19 +972,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -992,19 +992,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1012,19 +1012,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1032,19 +1032,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1052,7 +1052,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1061,10 +1061,10 @@
         <v>2</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F31" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1072,7 +1072,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1081,10 +1081,10 @@
         <v>2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F32" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1092,7 +1092,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1101,10 +1101,10 @@
         <v>2</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1112,7 +1112,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1121,10 +1121,10 @@
         <v>2</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1132,7 +1132,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1141,10 +1141,10 @@
         <v>2</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F35" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1152,7 +1152,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1161,10 +1161,10 @@
         <v>2</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1172,7 +1172,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1181,10 +1181,10 @@
         <v>2</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F37" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1192,7 +1192,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1201,10 +1201,10 @@
         <v>2</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F38" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1212,7 +1212,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1221,10 +1221,10 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F39" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1232,7 +1232,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -1241,10 +1241,10 @@
         <v>2</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1252,7 +1252,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1261,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1272,7 +1272,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -1281,10 +1281,10 @@
         <v>2</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F42" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1292,7 +1292,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -1301,10 +1301,10 @@
         <v>2</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F43" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1312,7 +1312,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1321,10 +1321,10 @@
         <v>2</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F44" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1332,7 +1332,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -1341,10 +1341,10 @@
         <v>2</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F45" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1352,7 +1352,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -1361,10 +1361,10 @@
         <v>2</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F46" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1372,7 +1372,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1381,10 +1381,10 @@
         <v>2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F47" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1392,7 +1392,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -1401,10 +1401,10 @@
         <v>2</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F48" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1412,7 +1412,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -1421,10 +1421,10 @@
         <v>2</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F49" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1432,7 +1432,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -1441,10 +1441,10 @@
         <v>2</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F50" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1452,7 +1452,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -1461,10 +1461,10 @@
         <v>2</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1472,7 +1472,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -1481,10 +1481,10 @@
         <v>2</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1492,7 +1492,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -1501,10 +1501,10 @@
         <v>2</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F53" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1512,7 +1512,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -1521,10 +1521,10 @@
         <v>2</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F54" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1532,19 +1532,19 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F55" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1552,7 +1552,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -1561,10 +1561,10 @@
         <v>2</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F56" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1572,7 +1572,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -1581,10 +1581,10 @@
         <v>2</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F57" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1592,7 +1592,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -1601,10 +1601,10 @@
         <v>2</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F58" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1612,7 +1612,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -1621,10 +1621,10 @@
         <v>2</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F59" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1632,7 +1632,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -1641,10 +1641,10 @@
         <v>2</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F60" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1652,7 +1652,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -1661,10 +1661,10 @@
         <v>2</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F61" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1672,7 +1672,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -1681,10 +1681,10 @@
         <v>2</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F62" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1692,7 +1692,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1701,10 +1701,10 @@
         <v>2</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F63" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1712,7 +1712,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -1721,10 +1721,10 @@
         <v>2</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1732,7 +1732,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -1741,10 +1741,10 @@
         <v>2</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F65" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1752,7 +1752,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -1761,10 +1761,10 @@
         <v>2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F66" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1772,7 +1772,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -1781,10 +1781,10 @@
         <v>2</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F67" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1792,19 +1792,19 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F68" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1812,19 +1812,19 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F69" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1832,19 +1832,19 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1852,19 +1852,19 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F71" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1872,19 +1872,19 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F72" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1892,19 +1892,19 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F73" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1912,19 +1912,19 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1932,19 +1932,19 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F75" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1952,19 +1952,19 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F76" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1972,19 +1972,19 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1992,19 +1992,19 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F78" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2012,19 +2012,19 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F79" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2032,19 +2032,19 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F80" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2052,19 +2052,19 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F81" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2072,19 +2072,19 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F82" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2092,19 +2092,19 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F83" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2112,19 +2112,19 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F84" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2132,19 +2132,19 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F85" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2152,19 +2152,19 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F86" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2172,19 +2172,19 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2192,19 +2192,19 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F88" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2212,19 +2212,19 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F89" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2232,19 +2232,19 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F90" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2252,19 +2252,19 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F91" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2272,16 +2272,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F92" s="4">
         <v>0</v>
@@ -2292,16 +2292,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="4">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="4">
         <v>0</v>
@@ -2332,16 +2332,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95" s="4">
         <v>0</v>
@@ -2352,16 +2352,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" s="4">
         <v>0</v>
@@ -2372,16 +2372,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97" s="4">
         <v>0</v>
@@ -2392,16 +2392,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F98" s="4">
         <v>0</v>
@@ -2412,16 +2412,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F99" s="4">
         <v>0</v>
@@ -2432,16 +2432,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F100" s="4">
         <v>0</v>
@@ -2452,16 +2452,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="4">
         <v>0</v>
@@ -2472,16 +2472,16 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
added sensor reading sumary
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/mannedShipTestOutput.xlsx
+++ b/shipClassTests/testResults/mannedShipTestOutput.xlsx
@@ -555,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -575,13 +575,13 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="4">
         <v>2</v>
@@ -595,13 +595,13 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
@@ -615,13 +615,13 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
@@ -635,13 +635,13 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="4">
         <v>2</v>
@@ -655,13 +655,13 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="4">
         <v>2</v>
@@ -675,13 +675,13 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
@@ -695,13 +695,13 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="4">
         <v>2</v>
@@ -715,13 +715,13 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -735,13 +735,13 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
@@ -755,13 +755,13 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="4">
         <v>2</v>
@@ -775,13 +775,13 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="4">
         <v>2</v>
@@ -792,16 +792,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="4">
         <v>2</v>
@@ -812,16 +812,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -832,16 +832,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
@@ -852,16 +852,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" s="4">
         <v>2</v>
@@ -872,16 +872,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="4">
         <v>2</v>
@@ -892,16 +892,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" s="4">
         <v>2</v>
@@ -912,16 +912,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="4">
         <v>2</v>
@@ -932,19 +932,19 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -952,19 +952,19 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -972,19 +972,19 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -992,19 +992,19 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1012,19 +1012,19 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1032,19 +1032,19 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1052,19 +1052,19 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F31" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1072,19 +1072,19 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F32" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1092,19 +1092,19 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1112,19 +1112,19 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F34" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1132,19 +1132,19 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F35" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1152,19 +1152,19 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F36" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1172,19 +1172,19 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F37" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1192,19 +1192,19 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F38" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1212,19 +1212,19 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F39" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1232,19 +1232,19 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F40" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1252,19 +1252,19 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1272,19 +1272,19 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F42" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1292,19 +1292,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1312,19 +1312,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1332,19 +1332,19 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1352,19 +1352,19 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1372,19 +1372,19 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1392,19 +1392,19 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F48" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1412,19 +1412,19 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F49" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1432,19 +1432,19 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F50" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1452,19 +1452,19 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F51" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1472,19 +1472,19 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F52" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1492,19 +1492,19 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F53" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1512,19 +1512,19 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F54" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1532,19 +1532,19 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F55" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1552,19 +1552,19 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F56" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1572,19 +1572,19 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F57" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1592,19 +1592,19 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F58" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1612,19 +1612,19 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F59" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1632,19 +1632,19 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F60" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1652,19 +1652,19 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F61" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1672,19 +1672,19 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F62" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1692,19 +1692,19 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F63" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1712,19 +1712,19 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F64" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1732,19 +1732,19 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F65" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1752,19 +1752,19 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F66" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1772,19 +1772,19 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F67" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1792,19 +1792,19 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
       <c r="D68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F68" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1812,19 +1812,19 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F69" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1832,19 +1832,19 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F70" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1852,19 +1852,19 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F71" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1872,19 +1872,19 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F72" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1892,19 +1892,19 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F73" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1912,19 +1912,19 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C74">
         <v>0</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F74" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1932,19 +1932,19 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F75" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1952,19 +1952,19 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C76">
         <v>0</v>
       </c>
       <c r="D76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F76" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1972,19 +1972,19 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F77" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1992,19 +1992,19 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F78" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2012,19 +2012,19 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F79" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2032,19 +2032,19 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F80" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2052,19 +2052,19 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F81" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2072,19 +2072,19 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F82" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2092,19 +2092,19 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F83" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2112,19 +2112,19 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F84" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2132,19 +2132,19 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F85" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2152,19 +2152,19 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C86">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F86" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2172,19 +2172,19 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F87" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2192,19 +2192,19 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F88" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2212,19 +2212,19 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C89">
         <v>0</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F89" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2232,19 +2232,19 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C90">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F90" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2252,19 +2252,19 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C91">
         <v>0</v>
       </c>
       <c r="D91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E91">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F91" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2272,16 +2272,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C92">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F92" s="4">
         <v>0</v>
@@ -2292,16 +2292,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C93">
         <v>0</v>
       </c>
       <c r="D93">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F93" s="4">
         <v>0</v>
@@ -2312,16 +2312,16 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94" s="4">
         <v>0</v>
@@ -2332,16 +2332,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C95">
         <v>0</v>
       </c>
       <c r="D95">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" s="4">
         <v>0</v>
@@ -2352,16 +2352,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F96" s="4">
         <v>0</v>
@@ -2372,16 +2372,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C97">
         <v>0</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F97" s="4">
         <v>0</v>
@@ -2392,16 +2392,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C98">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" s="4">
         <v>0</v>
@@ -2412,16 +2412,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99">
         <v>0</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F99" s="4">
         <v>0</v>
@@ -2432,16 +2432,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C100">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F100" s="4">
         <v>0</v>
@@ -2452,16 +2452,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101">
         <v>0</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F101" s="4">
         <v>0</v>
@@ -2472,16 +2472,16 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102">
         <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
added summary of readings
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/mannedShipTestOutput.xlsx
+++ b/shipClassTests/testResults/mannedShipTestOutput.xlsx
@@ -552,19 +552,19 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -572,19 +572,19 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -592,19 +592,19 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -612,19 +612,19 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -632,19 +632,19 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -652,19 +652,19 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -672,19 +672,19 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -692,19 +692,19 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -712,19 +712,19 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -732,19 +732,19 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -752,19 +752,19 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -772,19 +772,19 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F17" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -792,19 +792,19 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F18" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -812,19 +812,19 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -832,19 +832,19 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -852,19 +852,19 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
       <c r="F21" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -872,19 +872,19 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -892,19 +892,19 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -912,19 +912,19 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -935,10 +935,10 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -955,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -975,10 +975,10 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -995,10 +995,10 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1015,10 +1015,10 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1035,10 +1035,10 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1055,10 +1055,10 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -1075,10 +1075,10 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -1095,10 +1095,10 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -1115,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1135,10 +1135,10 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1155,10 +1155,10 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1175,10 +1175,10 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1195,10 +1195,10 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1255,10 +1255,10 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1275,10 +1275,10 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -1295,10 +1295,10 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -1315,10 +1315,10 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1335,10 +1335,10 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -1355,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -1375,10 +1375,10 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1395,10 +1395,10 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -1415,10 +1415,10 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -1435,10 +1435,10 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -1455,10 +1455,10 @@
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -1475,10 +1475,10 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -1495,10 +1495,10 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -1515,10 +1515,10 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -1535,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -1555,10 +1555,10 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -1575,10 +1575,10 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -1595,10 +1595,10 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -1615,10 +1615,10 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -1635,10 +1635,10 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -1655,10 +1655,10 @@
         <v>0</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E61">
         <v>0</v>
@@ -1675,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -1695,10 +1695,10 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -1715,10 +1715,10 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -1735,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -1755,10 +1755,10 @@
         <v>0</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -1775,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -1795,10 +1795,10 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -1815,10 +1815,10 @@
         <v>0</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -1835,10 +1835,10 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -1855,10 +1855,10 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -1875,10 +1875,10 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -1895,10 +1895,10 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -1915,10 +1915,10 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -1935,10 +1935,10 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -1955,10 +1955,10 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -1975,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -1995,10 +1995,10 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -2015,10 +2015,10 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -2035,10 +2035,10 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -2098,7 +2098,7 @@
         <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -2118,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86">
         <v>0</v>

</xml_diff>